<commit_message>
Work on reading and writing grade tables (xlsx)
</commit_message>
<xml_diff>
--- a/TESTDATA/testing/Noten_1/Noten_13.xlsx
+++ b/TESTDATA/testing/Noten_1/Noten_13.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -28,7 +28,10 @@
     <t xml:space="preserve">Noten</t>
   </si>
   <si>
-    <t xml:space="preserve">Tabelle erstellt am 2020-03-21 07:26</t>
+    <t xml:space="preserve">Tabelle erstellt am 2020-11-11 11:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+++</t>
   </si>
   <si>
     <t xml:space="preserve">Schuljahr</t>
@@ -67,10 +70,10 @@
     <t xml:space="preserve">keine Note</t>
   </si>
   <si>
-    <t xml:space="preserve">Halbjahr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">Anlass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Halbjahr</t>
   </si>
   <si>
     <t xml:space="preserve">t: </t>
@@ -83,6 +86,18 @@
   </si>
   <si>
     <t xml:space="preserve">Fach nicht gewählt / nicht erteilt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notendatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-01-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausgabedatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-01-29</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -382,7 +397,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,6 +416,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -528,17 +547,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.74"/>
@@ -546,8 +565,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="1.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="5" style="1" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="25" style="1" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1006" min="31" style="1" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1007" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1006" min="31" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1007" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -577,467 +596,525 @@
       <c r="S1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="6"/>
+      <c r="R3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="44.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="N4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="11" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="44.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="G8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="H8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="I8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="J8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-    </row>
-    <row r="7" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14" t="s">
+      <c r="K8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15" t="s">
+      <c r="L8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="M8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="N8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="O8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-    </row>
-    <row r="8" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+    <row r="9" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="L9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="17" t="s">
+      <c r="N9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="O9" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="B11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="17" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N9" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="O9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-    </row>
-    <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="F11" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="G11" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="17" t="s">
+      <c r="H11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="L11" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="17" t="s">
+      <c r="N11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="B12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+    </row>
+    <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+    </row>
+    <row r="14" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-    </row>
-    <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="O14" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+    </row>
+    <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="O11" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-    </row>
-    <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="17" t="s">
+      <c r="K15" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="O12" s="17" t="s">
+      <c r="L15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-    </row>
-    <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-    </row>
-    <row r="14" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="N15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+    </row>
     <row r="16" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1073,6 +1150,8 @@
     <row r="48" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="49" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B1:D1"/>
@@ -1086,7 +1165,7 @@
     <mergeCell ref="N4:S4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E9:AD50" type="list">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E11:AD52" type="list">
       <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*,/"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>